<commit_message>
Regex Counter For Query Data
</commit_message>
<xml_diff>
--- a/Sample_Dataset/Secondary_Data.xlsx
+++ b/Sample_Dataset/Secondary_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luislascano01/Documents/Sabadell/Covenants_Matching/AI_VLookUp/Sample_Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{90D383A3-A160-1041-BAD8-A07516BF0AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{90EE2C90-7DC9-AA43-A94D-20DF0D111CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="940" windowWidth="17040" windowHeight="21260" xr2:uid="{25B03F2D-6921-FE47-B100-68C77C13EED2}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="17040" windowHeight="21260" xr2:uid="{25B03F2D-6921-FE47-B100-68C77C13EED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Secondary_Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="234">
   <si>
     <t>Verify_ID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>1 - Financials</t>
-  </si>
-  <si>
     <t>Acme Corp</t>
   </si>
   <si>
@@ -716,6 +713,15 @@
   </si>
   <si>
     <t>10070  PB</t>
+  </si>
+  <si>
+    <t>10001 - Financials</t>
+  </si>
+  <si>
+    <t>10098 - Lorem</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
@@ -1576,56 +1582,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFB6895-9A04-6049-B5A1-FDE83B8B650E}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>10001</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -1633,16 +1646,19 @@
         <v>10002</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>10002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10003</v>
       </c>
@@ -1650,24 +1666,30 @@
         <v>10003</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>10003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10004</v>
       </c>
+      <c r="B5">
+        <v>10004</v>
+      </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10005</v>
       </c>
@@ -1675,27 +1697,33 @@
         <v>10005</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>10005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10006</v>
       </c>
+      <c r="B7">
+        <v>10006</v>
+      </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10007</v>
       </c>
@@ -1703,27 +1731,33 @@
         <v>10007</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>10007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10008</v>
       </c>
-      <c r="B9" t="s">
-        <v>226</v>
+      <c r="B9">
+        <v>10008</v>
       </c>
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10009</v>
       </c>
@@ -1731,24 +1765,30 @@
         <v>10009</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>10009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10010</v>
       </c>
+      <c r="B11">
+        <v>10010</v>
+      </c>
       <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10011</v>
       </c>
@@ -1756,30 +1796,36 @@
         <v>10011</v>
       </c>
       <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>10011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10012</v>
       </c>
+      <c r="B13">
+        <v>10012</v>
+      </c>
       <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10013</v>
       </c>
@@ -1787,13 +1833,16 @@
         <v>10013</v>
       </c>
       <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>10013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10014</v>
       </c>
@@ -1801,16 +1850,19 @@
         <v>10014</v>
       </c>
       <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>10014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10015</v>
       </c>
@@ -1818,27 +1870,33 @@
         <v>10015</v>
       </c>
       <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>38</v>
       </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>10015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10016</v>
       </c>
+      <c r="B17">
+        <v>10016</v>
+      </c>
       <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10017</v>
       </c>
@@ -1846,27 +1904,33 @@
         <v>10017</v>
       </c>
       <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>10017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10018</v>
       </c>
+      <c r="B19">
+        <v>10018</v>
+      </c>
       <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10019</v>
       </c>
@@ -1874,30 +1938,36 @@
         <v>10019</v>
       </c>
       <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>48</v>
       </c>
-      <c r="E20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>10019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10020</v>
       </c>
-      <c r="B21" t="s">
-        <v>230</v>
+      <c r="B21">
+        <v>10020</v>
       </c>
       <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
         <v>50</v>
       </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>10021</v>
       </c>
@@ -1905,27 +1975,33 @@
         <v>10021</v>
       </c>
       <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
         <v>52</v>
       </c>
-      <c r="E22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>10021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10022</v>
       </c>
+      <c r="B23">
+        <v>10022</v>
+      </c>
       <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10023</v>
       </c>
@@ -1933,13 +2009,16 @@
         <v>10023</v>
       </c>
       <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>10023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10024</v>
       </c>
@@ -1947,16 +2026,19 @@
         <v>10024</v>
       </c>
       <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
         <v>59</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>60</v>
       </c>
-      <c r="E25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>10024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10025</v>
       </c>
@@ -1964,27 +2046,33 @@
         <v>10025</v>
       </c>
       <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
         <v>62</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>63</v>
       </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>10025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10026</v>
       </c>
+      <c r="B27">
+        <v>10026</v>
+      </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10027</v>
       </c>
@@ -1992,30 +2080,36 @@
         <v>10027</v>
       </c>
       <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
         <v>66</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>67</v>
       </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>10027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10028</v>
       </c>
+      <c r="B29">
+        <v>10028</v>
+      </c>
       <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
         <v>69</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>70</v>
       </c>
-      <c r="E29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10029</v>
       </c>
@@ -2023,16 +2117,19 @@
         <v>10029</v>
       </c>
       <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
         <v>72</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>73</v>
       </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>10029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10030</v>
       </c>
@@ -2040,35 +2137,44 @@
         <v>10030</v>
       </c>
       <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" t="s">
         <v>75</v>
       </c>
-      <c r="E31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>10030</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10031</v>
       </c>
+      <c r="B32">
+        <v>10031</v>
+      </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>10032</v>
       </c>
+      <c r="B33">
+        <v>10032</v>
+      </c>
       <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" t="s">
         <v>78</v>
       </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>10033</v>
       </c>
@@ -2076,16 +2182,19 @@
         <v>10033</v>
       </c>
       <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
         <v>80</v>
       </c>
-      <c r="D34" t="s">
-        <v>81</v>
-      </c>
       <c r="E34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F34">
+        <v>10033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>10034</v>
       </c>
@@ -2093,27 +2202,33 @@
         <v>10034</v>
       </c>
       <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>83</v>
       </c>
-      <c r="E35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>10034</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>10035</v>
       </c>
+      <c r="B36">
+        <v>10035</v>
+      </c>
       <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
         <v>85</v>
       </c>
-      <c r="E36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10036</v>
       </c>
@@ -2121,16 +2236,19 @@
         <v>10036</v>
       </c>
       <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
         <v>87</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>88</v>
       </c>
-      <c r="E37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>10036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>10037</v>
       </c>
@@ -2138,44 +2256,53 @@
         <v>10037</v>
       </c>
       <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" t="s">
         <v>90</v>
       </c>
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
       <c r="E38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <v>10037</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>10038</v>
       </c>
+      <c r="B39">
+        <v>10038</v>
+      </c>
       <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
         <v>92</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>93</v>
       </c>
-      <c r="E39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>10039</v>
       </c>
+      <c r="B40">
+        <v>10039</v>
+      </c>
       <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
         <v>95</v>
       </c>
-      <c r="D40" t="s">
-        <v>96</v>
-      </c>
       <c r="E40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>10040</v>
       </c>
@@ -2183,24 +2310,30 @@
         <v>10040</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="F41">
+        <v>10040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>10041</v>
       </c>
+      <c r="B42">
+        <v>10041</v>
+      </c>
       <c r="C42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" t="s">
         <v>98</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>99</v>
       </c>
-      <c r="E42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>10042</v>
       </c>
@@ -2208,61 +2341,73 @@
         <v>10042</v>
       </c>
       <c r="C43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
         <v>101</v>
       </c>
-      <c r="D43" t="s">
-        <v>102</v>
-      </c>
       <c r="E43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="F43">
+        <v>10042</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>10043</v>
       </c>
-      <c r="B44" t="s">
-        <v>229</v>
+      <c r="B44">
+        <v>10043</v>
       </c>
       <c r="C44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" t="s">
         <v>103</v>
       </c>
-      <c r="D44" t="s">
-        <v>104</v>
-      </c>
       <c r="E44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>10044</v>
       </c>
       <c r="B45">
+        <v>10044</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="E45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>10045</v>
       </c>
+      <c r="B46">
+        <v>10045</v>
+      </c>
       <c r="C46" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" t="s">
         <v>107</v>
       </c>
-      <c r="D46" t="s">
-        <v>108</v>
-      </c>
       <c r="E46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>10046</v>
       </c>
@@ -2270,10 +2415,13 @@
         <v>10046</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F47">
+        <v>10046</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>10047</v>
       </c>
@@ -2281,16 +2429,19 @@
         <v>10047</v>
       </c>
       <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="s">
         <v>110</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>111</v>
       </c>
-      <c r="E48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>10047</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>10048</v>
       </c>
@@ -2298,44 +2449,53 @@
         <v>10048</v>
       </c>
       <c r="C49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
         <v>113</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>114</v>
       </c>
-      <c r="E49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>10048</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>10049</v>
       </c>
+      <c r="B50">
+        <v>10049</v>
+      </c>
       <c r="C50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
         <v>116</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>117</v>
       </c>
-      <c r="E50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>10050</v>
       </c>
+      <c r="B51">
+        <v>10050</v>
+      </c>
       <c r="C51" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" t="s">
         <v>119</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>120</v>
       </c>
-      <c r="E51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>10051</v>
       </c>
@@ -2343,55 +2503,67 @@
         <v>10051</v>
       </c>
       <c r="C52" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="F52">
+        <v>10051</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>10052</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53">
+        <v>10052</v>
+      </c>
+      <c r="C53" t="s">
         <v>123</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>124</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>125</v>
       </c>
-      <c r="E53" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>10053</v>
       </c>
+      <c r="B54">
+        <v>10053</v>
+      </c>
       <c r="C54" t="s">
+        <v>126</v>
+      </c>
+      <c r="D54" t="s">
         <v>127</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>128</v>
       </c>
-      <c r="E54" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>10054</v>
       </c>
+      <c r="B55">
+        <v>10054</v>
+      </c>
       <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
         <v>130</v>
       </c>
-      <c r="D55" t="s">
-        <v>131</v>
-      </c>
       <c r="E55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>10055</v>
       </c>
@@ -2399,21 +2571,27 @@
         <v>10055</v>
       </c>
       <c r="C56" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="F56">
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>10056</v>
       </c>
+      <c r="B57">
+        <v>10056</v>
+      </c>
       <c r="C57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>10057</v>
       </c>
@@ -2421,16 +2599,19 @@
         <v>10057</v>
       </c>
       <c r="C58" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" t="s">
         <v>134</v>
       </c>
-      <c r="D58" t="s">
-        <v>135</v>
-      </c>
       <c r="E58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="F58">
+        <v>10057</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>10058</v>
       </c>
@@ -2438,24 +2619,30 @@
         <v>10058</v>
       </c>
       <c r="C59" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" t="s">
         <v>136</v>
       </c>
-      <c r="D59" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>10058</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>10059</v>
       </c>
+      <c r="B60">
+        <v>10059</v>
+      </c>
       <c r="C60" t="s">
+        <v>137</v>
+      </c>
+      <c r="E60" t="s">
         <v>138</v>
       </c>
-      <c r="E60" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>10060</v>
       </c>
@@ -2463,16 +2650,19 @@
         <v>10060</v>
       </c>
       <c r="C61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="s">
         <v>140</v>
       </c>
-      <c r="D61" t="s">
-        <v>141</v>
-      </c>
       <c r="E61" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="F61">
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>10061</v>
       </c>
@@ -2480,16 +2670,19 @@
         <v>10061</v>
       </c>
       <c r="C62" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" t="s">
-        <v>143</v>
-      </c>
       <c r="E62" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F62">
+        <v>10061</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>10062</v>
       </c>
@@ -2497,55 +2690,67 @@
         <v>10062</v>
       </c>
       <c r="C63" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" t="s">
         <v>144</v>
       </c>
-      <c r="E63" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>10062</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>10063</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64">
+        <v>10063</v>
+      </c>
+      <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>147</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>148</v>
       </c>
-      <c r="E64" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>10064</v>
       </c>
+      <c r="B65">
+        <v>10064</v>
+      </c>
       <c r="C65" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" t="s">
         <v>150</v>
       </c>
-      <c r="D65" t="s">
-        <v>151</v>
-      </c>
       <c r="E65" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>10065</v>
       </c>
+      <c r="B66">
+        <v>10065</v>
+      </c>
       <c r="C66" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" t="s">
         <v>152</v>
       </c>
-      <c r="E66" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>10066</v>
       </c>
@@ -2553,30 +2758,36 @@
         <v>10066</v>
       </c>
       <c r="C67" t="s">
+        <v>153</v>
+      </c>
+      <c r="D67" t="s">
         <v>154</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>155</v>
       </c>
-      <c r="E67" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>10066</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>10067</v>
       </c>
+      <c r="B68">
+        <v>10067</v>
+      </c>
       <c r="C68" t="s">
+        <v>156</v>
+      </c>
+      <c r="D68" t="s">
         <v>157</v>
       </c>
-      <c r="D68" t="s">
-        <v>158</v>
-      </c>
       <c r="E68" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>10068</v>
       </c>
@@ -2584,13 +2795,16 @@
         <v>10068</v>
       </c>
       <c r="C69" t="s">
+        <v>158</v>
+      </c>
+      <c r="E69" t="s">
         <v>159</v>
       </c>
-      <c r="E69" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>10068</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>10069</v>
       </c>
@@ -2598,58 +2812,70 @@
         <v>10069</v>
       </c>
       <c r="C70" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" t="s">
         <v>161</v>
       </c>
-      <c r="D70" t="s">
-        <v>162</v>
-      </c>
       <c r="E70" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="F70">
+        <v>10069</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>10070</v>
       </c>
-      <c r="B71" t="s">
-        <v>231</v>
+      <c r="B71">
+        <v>10070</v>
       </c>
       <c r="C71" t="s">
+        <v>162</v>
+      </c>
+      <c r="E71" t="s">
         <v>163</v>
       </c>
-      <c r="E71" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>10071</v>
       </c>
+      <c r="B72">
+        <v>10071</v>
+      </c>
       <c r="C72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" t="s">
         <v>165</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>166</v>
       </c>
-      <c r="E72" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>10072</v>
       </c>
+      <c r="B73">
+        <v>10072</v>
+      </c>
       <c r="C73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D73" t="s">
         <v>168</v>
       </c>
-      <c r="D73" t="s">
-        <v>169</v>
-      </c>
       <c r="E73" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>10073</v>
       </c>
@@ -2657,38 +2883,47 @@
         <v>10073</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <v>10073</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>10074</v>
       </c>
+      <c r="B75">
+        <v>10074</v>
+      </c>
       <c r="C75" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" t="s">
         <v>171</v>
       </c>
-      <c r="D75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>10075</v>
       </c>
+      <c r="B76">
+        <v>10075</v>
+      </c>
       <c r="C76" t="s">
+        <v>172</v>
+      </c>
+      <c r="D76" t="s">
         <v>173</v>
       </c>
-      <c r="D76" t="s">
-        <v>174</v>
-      </c>
       <c r="E76" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>10076</v>
       </c>
@@ -2696,58 +2931,70 @@
         <v>10076</v>
       </c>
       <c r="C77" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" t="s">
         <v>175</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>176</v>
       </c>
-      <c r="E77" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>10076</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>10077</v>
       </c>
-      <c r="B78" t="s">
-        <v>227</v>
+      <c r="B78">
+        <v>10077</v>
       </c>
       <c r="C78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E78" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="F78" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>10078</v>
       </c>
+      <c r="B79">
+        <v>10078</v>
+      </c>
       <c r="C79" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" t="s">
         <v>179</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>180</v>
       </c>
-      <c r="E79" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>10079</v>
       </c>
-      <c r="B80" t="s">
-        <v>228</v>
+      <c r="B80">
+        <v>10079</v>
       </c>
       <c r="C80" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" t="s">
         <v>182</v>
       </c>
-      <c r="D80" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>10080</v>
       </c>
@@ -2755,16 +3002,19 @@
         <v>10080</v>
       </c>
       <c r="C81" t="s">
+        <v>183</v>
+      </c>
+      <c r="D81" t="s">
         <v>184</v>
       </c>
-      <c r="D81" t="s">
-        <v>185</v>
-      </c>
       <c r="E81" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="F81">
+        <v>10080</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>10081</v>
       </c>
@@ -2772,27 +3022,33 @@
         <v>10081</v>
       </c>
       <c r="C82" t="s">
+        <v>185</v>
+      </c>
+      <c r="E82" t="s">
         <v>186</v>
       </c>
-      <c r="E82" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>10081</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>10082</v>
       </c>
+      <c r="B83">
+        <v>10082</v>
+      </c>
       <c r="C83" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" t="s">
         <v>188</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>189</v>
       </c>
-      <c r="E83" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>10083</v>
       </c>
@@ -2800,27 +3056,33 @@
         <v>10083</v>
       </c>
       <c r="C84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E84" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="F84">
+        <v>10083</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>10084</v>
       </c>
+      <c r="B85">
+        <v>10084</v>
+      </c>
       <c r="C85" t="s">
+        <v>191</v>
+      </c>
+      <c r="D85" t="s">
         <v>192</v>
       </c>
-      <c r="D85" t="s">
-        <v>193</v>
-      </c>
       <c r="E85" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>10085</v>
       </c>
@@ -2828,13 +3090,16 @@
         <v>10085</v>
       </c>
       <c r="C86" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E86" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F86">
+        <v>10085</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>10086</v>
       </c>
@@ -2842,16 +3107,19 @@
         <v>10086</v>
       </c>
       <c r="C87" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s">
         <v>195</v>
       </c>
-      <c r="D87" t="s">
-        <v>196</v>
-      </c>
       <c r="E87" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F87">
+        <v>10086</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>10087</v>
       </c>
@@ -2859,27 +3127,33 @@
         <v>10087</v>
       </c>
       <c r="C88" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" t="s">
         <v>197</v>
       </c>
-      <c r="D88" t="s">
-        <v>198</v>
-      </c>
       <c r="E88" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F88">
+        <v>10087</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>10088</v>
       </c>
+      <c r="B89">
+        <v>10088</v>
+      </c>
       <c r="C89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E89" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>10089</v>
       </c>
@@ -2887,13 +3161,16 @@
         <v>10089</v>
       </c>
       <c r="C90" t="s">
+        <v>199</v>
+      </c>
+      <c r="D90" t="s">
         <v>200</v>
       </c>
-      <c r="D90" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>10089</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>10090</v>
       </c>
@@ -2901,16 +3178,19 @@
         <v>10090</v>
       </c>
       <c r="C91" t="s">
+        <v>201</v>
+      </c>
+      <c r="D91" t="s">
         <v>202</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>203</v>
       </c>
-      <c r="E91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>10090</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>10091</v>
       </c>
@@ -2918,27 +3198,33 @@
         <v>10091</v>
       </c>
       <c r="C92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E92" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F92">
+        <v>10091</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>10092</v>
       </c>
+      <c r="B93">
+        <v>10092</v>
+      </c>
       <c r="C93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E93" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>10093</v>
       </c>
@@ -2946,16 +3232,19 @@
         <v>10093</v>
       </c>
       <c r="C94" t="s">
+        <v>205</v>
+      </c>
+      <c r="D94" t="s">
         <v>206</v>
       </c>
-      <c r="D94" t="s">
-        <v>207</v>
-      </c>
       <c r="E94" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="F94">
+        <v>10093</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>10094</v>
       </c>
@@ -2963,24 +3252,30 @@
         <v>10094</v>
       </c>
       <c r="C95" t="s">
+        <v>207</v>
+      </c>
+      <c r="E95" t="s">
         <v>208</v>
       </c>
-      <c r="E95" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>10094</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>10095</v>
       </c>
+      <c r="B96">
+        <v>10095</v>
+      </c>
       <c r="C96" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" t="s">
         <v>210</v>
       </c>
-      <c r="D96" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>10096</v>
       </c>
@@ -2988,27 +3283,33 @@
         <v>10096</v>
       </c>
       <c r="C97" t="s">
+        <v>211</v>
+      </c>
+      <c r="E97" t="s">
         <v>212</v>
       </c>
-      <c r="E97" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>10096</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>10097</v>
       </c>
+      <c r="B98">
+        <v>10097</v>
+      </c>
       <c r="C98" t="s">
+        <v>213</v>
+      </c>
+      <c r="D98" t="s">
         <v>214</v>
       </c>
-      <c r="D98" t="s">
-        <v>215</v>
-      </c>
       <c r="E98" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>10098</v>
       </c>
@@ -3016,52 +3317,64 @@
         <v>10098</v>
       </c>
       <c r="C99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E99" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F99" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>10099</v>
       </c>
+      <c r="B100">
+        <v>10099</v>
+      </c>
       <c r="C100" t="s">
+        <v>216</v>
+      </c>
+      <c r="D100" t="s">
         <v>217</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>218</v>
       </c>
-      <c r="E100" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>10100</v>
       </c>
+      <c r="B101">
+        <v>10100</v>
+      </c>
       <c r="C101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E101" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>10101</v>
       </c>
+      <c r="B102">
+        <v>10101</v>
+      </c>
       <c r="C102" t="s">
+        <v>223</v>
+      </c>
+      <c r="D102" t="s">
         <v>224</v>
       </c>
-      <c r="D102" t="s">
-        <v>225</v>
-      </c>
       <c r="E102" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>